<commit_message>
batch changes with log4j
</commit_message>
<xml_diff>
--- a/RestAssuredTest/src/test/resources/data/testData.xlsx
+++ b/RestAssuredTest/src/test/resources/data/testData.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AKandan1/git/Team2_TestingTurtles/RestAssuredTest/src/test/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5897E6FA-49DC-7B47-9CF1-870BA3A47E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F444CE-DEEA-7A4D-AC79-521027F8842F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="8080" windowWidth="32520" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="batch" sheetId="1" r:id="rId1"/>
+    <sheet name="hf" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>dataKey</t>
   </si>
@@ -46,9 +47,6 @@
     <t>batches</t>
   </si>
   <si>
-    <t>batchesss</t>
-  </si>
-  <si>
     <t>Get_ByBatchId_Valid</t>
   </si>
   <si>
@@ -70,26 +68,50 @@
     <t>batchId</t>
   </si>
   <si>
-    <t>batchIds</t>
-  </si>
-  <si>
     <t>batchName</t>
   </si>
   <si>
-    <t>batchNames</t>
-  </si>
-  <si>
     <t>program</t>
   </si>
   <si>
-    <t>programs</t>
+    <t>Post_ByBatchName_Invalid</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>Sdet</t>
+  </si>
+  <si>
+    <t>Post_ByBatchName_Missingfield</t>
+  </si>
+  <si>
+    <t>TestingTurtles_SDET_54781</t>
+  </si>
+  <si>
+    <t>BatchStatus</t>
+  </si>
+  <si>
+    <t>NoOfClasses</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>BatchDescription</t>
+  </si>
+  <si>
+    <t>SDET</t>
+  </si>
+  <si>
+    <t>Post_Batch_Valid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +145,24 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0451A5"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF098658"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,7 +186,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -160,6 +200,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -437,104 +486,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.83203125" style="1"/>
+    <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="18.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="45.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="45.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.5" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -542,4 +559,167 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2813D39-079A-C441-B8F0-FE4801F46DDC}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>11295</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding scenarios for assignment, logging
</commit_message>
<xml_diff>
--- a/RestAssuredTest/src/test/resources/data/testData.xlsx
+++ b/RestAssuredTest/src/test/resources/data/testData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="138">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -288,6 +288,9 @@
     <t>comments</t>
   </si>
   <si>
+    <t>dueDate</t>
+  </si>
+  <si>
     <t>pathAttachment1</t>
   </si>
   <si>
@@ -321,6 +324,9 @@
     <t>Testing for Assignment</t>
   </si>
   <si>
+    <t>2023-07-29T22:00:04.964+00:00</t>
+  </si>
+  <si>
     <t>pathfile1.json</t>
   </si>
   <si>
@@ -339,15 +345,48 @@
     <t>Post_Assignment_Existing</t>
   </si>
   <si>
-    <t>&lt;set in code&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">Assignment already exists with given Name : </t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
+    <t>Post_Assignment_MissingAssignmentName</t>
+  </si>
+  <si>
+    <t>Assignment Name is mandatory</t>
+  </si>
+  <si>
+    <t>Post_Assignment_MissingDueDate</t>
+  </si>
+  <si>
+    <t>Due Date is mandatory</t>
+  </si>
+  <si>
+    <t>Post_Assignment_MissingAssignmentDescription</t>
+  </si>
+  <si>
+    <t>Assignment Description is mandatory</t>
+  </si>
+  <si>
+    <t>Post_Assignment_MissingBatchId</t>
+  </si>
+  <si>
+    <t>Batch ID is mandatory</t>
+  </si>
+  <si>
+    <t>Post_Assignment_MissingCreatedBy</t>
+  </si>
+  <si>
+    <t>Created By is mandatory</t>
+  </si>
+  <si>
+    <t>Post_Assignment_MissingGraderId</t>
+  </si>
+  <si>
+    <t>Grader ID is mandatory</t>
+  </si>
+  <si>
     <t>Delete_Assignment_ValidId</t>
   </si>
   <si>
@@ -370,6 +409,36 @@
   </si>
   <si>
     <t xml:space="preserve">Batch not found with Id : </t>
+  </si>
+  <si>
+    <t>Put_Assignment_ValidId</t>
+  </si>
+  <si>
+    <t>SDET SQL Assignment Update</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Put_Assignment_InvalidId</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingAssignmentName</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingDueDate</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingAssignmentDescription</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingBatchId</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingCreatedBy</t>
+  </si>
+  <si>
+    <t>Put_Assignment_MissingGraderId</t>
   </si>
   <si>
     <t>Get_All_Valid</t>
@@ -418,7 +487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -472,13 +541,23 @@
       <name val="Menlo Regular"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="18"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
       <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="18"/>
+      <color indexed="19"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="20"/>
       <name val="Menlo Regular"/>
     </font>
   </fonts>
@@ -673,7 +752,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -803,6 +882,12 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -812,7 +897,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -841,6 +926,8 @@
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff2a00ff"/>
       <rgbColor rgb="ff0451a5"/>
+      <rgbColor rgb="ff00cdb2"/>
+      <rgbColor rgb="ffd3d3d3"/>
       <rgbColor rgb="ff098658"/>
     </indexedColors>
   </colors>
@@ -2818,18 +2905,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30" style="41" customWidth="1"/>
+    <col min="1" max="1" width="54" style="41" customWidth="1"/>
     <col min="2" max="2" width="38.5" style="41" customWidth="1"/>
     <col min="3" max="3" width="24" style="41" customWidth="1"/>
     <col min="4" max="4" width="27.5" style="41" customWidth="1"/>
-    <col min="5" max="11" width="18" style="41" customWidth="1"/>
-    <col min="12" max="16384" width="9.85156" style="41" customWidth="1"/>
+    <col min="5" max="10" width="18" style="41" customWidth="1"/>
+    <col min="11" max="11" width="44.8516" style="41" customWidth="1"/>
+    <col min="12" max="12" width="18" style="41" customWidth="1"/>
+    <col min="13" max="16384" width="9.85156" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -2866,252 +2955,787 @@
       <c r="K1" t="s" s="26">
         <v>80</v>
       </c>
+      <c r="L1" t="s" s="26">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="28">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s" s="28">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s" s="28">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s" s="28">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s" s="28">
         <v>85</v>
       </c>
+      <c r="E2" t="s" s="42">
+        <v>86</v>
+      </c>
       <c r="F2" t="s" s="28">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s" s="28">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H2" t="s" s="28">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s" s="28">
-        <v>89</v>
-      </c>
-      <c r="J2" s="28"/>
+        <v>90</v>
+      </c>
+      <c r="J2" t="s" s="28">
+        <v>91</v>
+      </c>
       <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="28">
+        <v>92</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E3" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F3" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G3" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I3" t="s" s="28">
         <v>90</v>
       </c>
-      <c r="B3" t="s" s="28">
+      <c r="J3" t="s" s="28">
         <v>91</v>
       </c>
-      <c r="C3" t="s" s="28">
+      <c r="K3" t="s" s="43">
+        <v>93</v>
+      </c>
+      <c r="L3" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" t="s" s="44">
+        <v>95</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F4" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I4" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K4" t="s" s="43">
+        <v>96</v>
+      </c>
+      <c r="L4" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="44">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s" s="28">
         <v>83</v>
       </c>
-      <c r="D3" t="s" s="28">
+      <c r="C5" t="s" s="28">
         <v>84</v>
       </c>
-      <c r="E3" t="s" s="28">
+      <c r="D5" t="s" s="28">
         <v>85</v>
       </c>
-      <c r="F3" t="s" s="28">
+      <c r="E5" s="42"/>
+      <c r="F5" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H5" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I5" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J5" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K5" t="s" s="43">
+        <v>98</v>
+      </c>
+      <c r="L5" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="44">
+        <v>99</v>
+      </c>
+      <c r="B6" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s" s="42">
         <v>86</v>
       </c>
-      <c r="G3" t="s" s="28">
+      <c r="F6" t="s" s="28">
         <v>87</v>
       </c>
-      <c r="H3" t="s" s="28">
+      <c r="G6" t="s" s="28">
         <v>88</v>
       </c>
-      <c r="I3" t="s" s="28">
+      <c r="H6" t="s" s="28">
         <v>89</v>
       </c>
-      <c r="J3" t="s" s="42">
-        <v>92</v>
-      </c>
-      <c r="K3" t="s" s="28">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="28">
+      <c r="I6" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J6" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K6" t="s" s="43">
+        <v>100</v>
+      </c>
+      <c r="L6" t="s" s="28">
         <v>94</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" t="s" s="42">
-        <v>95</v>
-      </c>
-      <c r="K4" t="s" s="28">
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" t="s" s="44">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D7" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G7" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H7" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I7" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J7" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K7" t="s" s="43">
+        <v>102</v>
+      </c>
+      <c r="L7" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" t="s" s="44">
+        <v>103</v>
+      </c>
+      <c r="B8" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C8" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E8" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F8" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G8" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J8" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K8" t="s" s="43">
+        <v>104</v>
+      </c>
+      <c r="L8" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" t="s" s="42">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F9" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H9" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I9" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J9" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K9" t="s" s="43">
+        <v>106</v>
+      </c>
+      <c r="L9" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" t="s" s="28">
+        <v>107</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" t="s" s="43">
+        <v>108</v>
+      </c>
+      <c r="L10" t="s" s="28">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1">
+      <c r="A11" t="s" s="28">
+        <v>110</v>
+      </c>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" t="s" s="43">
+        <v>111</v>
+      </c>
+      <c r="L11" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1">
+      <c r="A12" t="s" s="28">
+        <v>112</v>
+      </c>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" t="s" s="43">
+        <v>111</v>
+      </c>
+      <c r="L12" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1">
+      <c r="A13" t="s" s="28">
+        <v>113</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" t="s" s="43">
+        <v>114</v>
+      </c>
+      <c r="L13" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1">
+      <c r="A14" t="s" s="28">
+        <v>115</v>
+      </c>
+      <c r="B14" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C14" t="s" s="28">
+        <v>116</v>
+      </c>
+      <c r="D14" t="s" s="28">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G14" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H14" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J14" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="A15" t="s" s="28">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C15" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D15" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G15" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I15" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J15" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K15" t="s" s="43">
+        <v>111</v>
+      </c>
+      <c r="L15" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1">
+      <c r="A16" t="s" s="44">
+        <v>119</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E16" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G16" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J16" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K16" t="s" s="43">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="28">
-        <v>97</v>
-      </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" t="s" s="42">
+      <c r="L16" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1">
+      <c r="A17" t="s" s="44">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D17" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E17" s="42"/>
+      <c r="F17" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G17" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I17" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J17" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K17" t="s" s="43">
         <v>98</v>
       </c>
-      <c r="K5" t="s" s="28">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="28">
-        <v>99</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" t="s" s="42">
-        <v>98</v>
-      </c>
-      <c r="K6" t="s" s="28">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" t="s" s="28">
+      <c r="L17" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1">
+      <c r="A18" t="s" s="44">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G18" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H18" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I18" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J18" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K18" t="s" s="43">
         <v>100</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" t="s" s="42">
-        <v>101</v>
-      </c>
-      <c r="K7" t="s" s="28">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-    </row>
-    <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-    </row>
-    <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-    </row>
-    <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-    </row>
-    <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-    </row>
-    <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="38"/>
-    </row>
-    <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
+      <c r="L18" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1">
+      <c r="A19" t="s" s="44">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G19" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I19" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J19" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K19" t="s" s="43">
+        <v>102</v>
+      </c>
+      <c r="L19" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1">
+      <c r="A20" t="s" s="44">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I20" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J20" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K20" t="s" s="43">
+        <v>104</v>
+      </c>
+      <c r="L20" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1">
+      <c r="A21" t="s" s="42">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s" s="28">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s" s="28">
+        <v>84</v>
+      </c>
+      <c r="D21" t="s" s="28">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s" s="42">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s" s="28">
+        <v>87</v>
+      </c>
+      <c r="G21" t="s" s="28">
+        <v>88</v>
+      </c>
+      <c r="H21" t="s" s="28">
+        <v>89</v>
+      </c>
+      <c r="I21" t="s" s="28">
+        <v>90</v>
+      </c>
+      <c r="J21" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="K21" t="s" s="43">
+        <v>106</v>
+      </c>
+      <c r="L21" t="s" s="28">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+    </row>
+    <row r="23" ht="13.5" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+    </row>
+    <row r="24" ht="13.5" customHeight="1">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+    </row>
+    <row r="27" ht="13.5" customHeight="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+    </row>
+    <row r="28" ht="13.5" customHeight="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+    </row>
+    <row r="29" ht="13.5" customHeight="1">
+      <c r="A29" s="20"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511806" footer="0.511806"/>
@@ -3130,112 +3754,112 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35.6719" style="44" customWidth="1"/>
-    <col min="2" max="2" width="30.8516" style="44" customWidth="1"/>
-    <col min="3" max="7" width="10.8516" style="44" customWidth="1"/>
-    <col min="8" max="16384" width="10.8516" style="44" customWidth="1"/>
+    <col min="1" max="1" width="35.6719" style="46" customWidth="1"/>
+    <col min="2" max="2" width="30.8516" style="46" customWidth="1"/>
+    <col min="3" max="7" width="10.8516" style="46" customWidth="1"/>
+    <col min="8" max="16384" width="10.8516" style="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
       <c r="A1" t="s" s="28">
-        <v>102</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+        <v>125</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
       <c r="G1" t="s" s="28">
         <v>29</v>
       </c>
     </row>
     <row r="2" ht="15" customHeight="1">
       <c r="A2" t="s" s="28">
-        <v>103</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+        <v>126</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
       <c r="G2" t="s" s="28">
         <v>29</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" t="s" s="28">
-        <v>104</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+        <v>127</v>
+      </c>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
       <c r="G3" t="s" s="28">
-        <v>105</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" t="s" s="28">
-        <v>106</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
+        <v>129</v>
+      </c>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
       <c r="G4" t="s" s="28">
-        <v>105</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" t="s" s="28">
-        <v>107</v>
-      </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
+        <v>130</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
       <c r="G5" t="s" s="28">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" t="s" s="28">
-        <v>109</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
+        <v>132</v>
+      </c>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
       <c r="G6" t="s" s="28">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" t="s" s="28">
-        <v>110</v>
-      </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+        <v>133</v>
+      </c>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
       <c r="G7" t="s" s="28">
         <v>8</v>
       </c>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" t="s" s="28">
-        <v>111</v>
-      </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+        <v>134</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
       <c r="G8" t="s" s="28">
         <v>8</v>
       </c>
@@ -3256,16 +3880,16 @@
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
-      <c r="G10" s="45"/>
+      <c r="G10" s="47"/>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" t="s" s="28">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s" s="29">
-        <v>113</v>
-      </c>
-      <c r="C11" s="46">
+        <v>136</v>
+      </c>
+      <c r="C11" s="48">
         <v>11295</v>
       </c>
       <c r="D11" t="s" s="30">
@@ -3283,7 +3907,7 @@
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" t="s" s="28">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B12" s="35"/>
       <c r="C12" s="35"/>

</xml_diff>